<commit_message>
Register and ALU updates
</commit_message>
<xml_diff>
--- a/InternalComponentListing.xlsx
+++ b/InternalComponentListing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">CID</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t xml:space="preserve">4 x 256 bit addressable register group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC11BALU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Bit ALU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Bit ALU. OPS: ADD, SUB, INC, DEC, AND, OR, NOT, XOR</t>
   </si>
 </sst>
 </file>
@@ -363,10 +372,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ14"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -574,6 +583,20 @@
         <v>42</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>45238</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Built part of ALU
</commit_message>
<xml_diff>
--- a/InternalComponentListing.xlsx
+++ b/InternalComponentListing.xlsx
@@ -151,13 +151,13 @@
     <t xml:space="preserve">4 x 256 bit addressable register group</t>
   </si>
   <si>
-    <t xml:space="preserve">JC11BALU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-Bit ALU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-Bit ALU. OPS: ADD, SUB, INC, DEC, AND, OR, NOT, XOR</t>
+    <t xml:space="preserve">JC11BALUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Bit ALU Part A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Bit ALU. OPS: ADD, SUB, NOR, NAND, AND, OR, NOT, XOR</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>